<commit_message>
update data for chirality
</commit_message>
<xml_diff>
--- a/data/par/1.xlsx
+++ b/data/par/1.xlsx
@@ -481,799 +481,799 @@
         <v>0</v>
       </c>
       <c r="B7" t="n">
-        <v>9.357104999999999e-09</v>
+        <v>0.0001359526</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.107006311416626</v>
+        <v>0.1050059795379639</v>
       </c>
       <c r="B8" t="n">
-        <v>9.3807e-09</v>
+        <v>0.0001360431</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2080121040344238</v>
+        <v>0.2010114192962646</v>
       </c>
       <c r="B9" t="n">
-        <v>9.463204000000001e-09</v>
+        <v>0.000135963</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.3040175437927246</v>
+        <v>0.3100178241729736</v>
       </c>
       <c r="B10" t="n">
-        <v>9.352661999999999e-09</v>
+        <v>0.0001360518</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.4050233364105225</v>
+        <v>0.4000227451324463</v>
       </c>
       <c r="B11" t="n">
-        <v>9.527472e-09</v>
+        <v>0.0001359725</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5090291500091553</v>
+        <v>0.5080287456512451</v>
       </c>
       <c r="B12" t="n">
-        <v>9.381918e-09</v>
+        <v>0.0001360137</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.6020345687866211</v>
+        <v>0.610034704208374</v>
       </c>
       <c r="B13" t="n">
-        <v>9.430238e-09</v>
+        <v>0.000135981</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.70404052734375</v>
+        <v>0.7080404758453369</v>
       </c>
       <c r="B14" t="n">
-        <v>9.443003e-09</v>
+        <v>0.000136022</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.8070461750030518</v>
+        <v>0.8160464763641357</v>
       </c>
       <c r="B15" t="n">
-        <v>9.504716e-09</v>
+        <v>0.0001360678</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.9010517597198486</v>
+        <v>0.9100520610809326</v>
       </c>
       <c r="B16" t="n">
-        <v>9.311866e-09</v>
+        <v>0.0001360378</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1.004057645797729</v>
+        <v>1.008057594299316</v>
       </c>
       <c r="B17" t="n">
-        <v>9.353858e-09</v>
+        <v>0.0001360517</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.106063365936279</v>
+        <v>1.116063594818115</v>
       </c>
       <c r="B18" t="n">
-        <v>9.50583e-09</v>
+        <v>0.0001360386</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.206068992614746</v>
+        <v>1.212069272994995</v>
       </c>
       <c r="B19" t="n">
-        <v>9.332274e-09</v>
+        <v>0.0001359773</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1.308074951171875</v>
+        <v>1.301074266433716</v>
       </c>
       <c r="B20" t="n">
-        <v>9.525528e-09</v>
+        <v>0.0001359701</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.40008020401001</v>
+        <v>1.407080411911011</v>
       </c>
       <c r="B21" t="n">
-        <v>9.293269999999999e-09</v>
+        <v>0.0001359875</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>1.501085996627808</v>
+        <v>1.509086132049561</v>
       </c>
       <c r="B22" t="n">
-        <v>9.300108e-09</v>
+        <v>0.0001360215</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>1.601091623306274</v>
+        <v>1.609091997146606</v>
       </c>
       <c r="B23" t="n">
-        <v>9.244176e-09</v>
+        <v>0.0001359827</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1.704097747802734</v>
+        <v>1.718098163604736</v>
       </c>
       <c r="B24" t="n">
-        <v>9.395528e-09</v>
+        <v>0.0001360192</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1.805103540420532</v>
+        <v>1.80910325050354</v>
       </c>
       <c r="B25" t="n">
-        <v>9.535156000000001e-09</v>
+        <v>0.0001359978</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1.908109426498413</v>
+        <v>1.909108877182007</v>
       </c>
       <c r="B26" t="n">
-        <v>9.550115e-09</v>
+        <v>0.0001359223</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2.009114980697632</v>
+        <v>2.021115303039551</v>
       </c>
       <c r="B27" t="n">
-        <v>9.416182e-09</v>
+        <v>0.0001359185</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2.102120637893677</v>
+        <v>2.105120182037354</v>
       </c>
       <c r="B28" t="n">
-        <v>9.47615e-09</v>
+        <v>0.0001359303</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2.204126358032227</v>
+        <v>2.214126586914062</v>
       </c>
       <c r="B29" t="n">
-        <v>9.530781999999999e-09</v>
+        <v>0.0001359182</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2.307132244110107</v>
+        <v>2.32113242149353</v>
       </c>
       <c r="B30" t="n">
-        <v>9.562648e-09</v>
+        <v>0.0001359041</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2.406137943267822</v>
+        <v>2.402137279510498</v>
       </c>
       <c r="B31" t="n">
-        <v>9.470152e-09</v>
+        <v>0.0001359525</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2.506143569946289</v>
+        <v>2.515143632888794</v>
       </c>
       <c r="B32" t="n">
-        <v>9.398621e-09</v>
+        <v>0.0001359074</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2.605149030685425</v>
+        <v>2.621149778366089</v>
       </c>
       <c r="B33" t="n">
-        <v>9.516703e-09</v>
+        <v>0.0001359666</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2.705154895782471</v>
+        <v>2.701154232025146</v>
       </c>
       <c r="B34" t="n">
-        <v>9.420357000000001e-09</v>
+        <v>0.0001359406</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2.805160522460938</v>
+        <v>2.80616021156311</v>
       </c>
       <c r="B35" t="n">
-        <v>9.548699e-09</v>
+        <v>0.0001358876</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2.90916633605957</v>
+        <v>2.910166263580322</v>
       </c>
       <c r="B36" t="n">
-        <v>9.457281e-09</v>
+        <v>0.0001359217</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3.009172439575195</v>
+        <v>3.013172149658203</v>
       </c>
       <c r="B37" t="n">
-        <v>9.312536e-09</v>
+        <v>0.0001359247</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3.100177526473999</v>
+        <v>3.104177236557007</v>
       </c>
       <c r="B38" t="n">
-        <v>9.351129e-09</v>
+        <v>0.0001358966</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3.201183319091797</v>
+        <v>3.217183828353882</v>
       </c>
       <c r="B39" t="n">
-        <v>9.268853e-09</v>
+        <v>0.0001358994</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3.302189111709595</v>
+        <v>3.306189060211182</v>
       </c>
       <c r="B40" t="n">
-        <v>9.464543000000001e-09</v>
+        <v>0.0001358811</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>3.403194665908813</v>
+        <v>3.406194686889648</v>
       </c>
       <c r="B41" t="n">
-        <v>9.331952e-09</v>
+        <v>0.0001358694</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3.504200458526611</v>
+        <v>3.508200407028198</v>
       </c>
       <c r="B42" t="n">
-        <v>9.413164000000001e-09</v>
+        <v>0.0001358824</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>3.60620641708374</v>
+        <v>3.615206480026245</v>
       </c>
       <c r="B43" t="n">
-        <v>9.279662999999999e-09</v>
+        <v>0.0001358565</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>3.702211856842041</v>
+        <v>3.704211711883545</v>
       </c>
       <c r="B44" t="n">
-        <v>9.524651999999999e-09</v>
+        <v>0.0001359285</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>3.807218074798584</v>
+        <v>3.806217432022095</v>
       </c>
       <c r="B45" t="n">
-        <v>9.344632e-09</v>
+        <v>0.000135875</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>3.908223867416382</v>
+        <v>3.911223411560059</v>
       </c>
       <c r="B46" t="n">
-        <v>9.411901e-09</v>
+        <v>0.0001358861</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>4.009229421615601</v>
+        <v>4.003228902816772</v>
       </c>
       <c r="B47" t="n">
-        <v>9.430745e-09</v>
+        <v>0.0001358125</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>4.102234840393066</v>
+        <v>4.118235349655151</v>
       </c>
       <c r="B48" t="n">
-        <v>9.506005999999999e-09</v>
+        <v>0.0001357939</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>4.205240726470947</v>
+        <v>4.200240135192871</v>
       </c>
       <c r="B49" t="n">
-        <v>9.518033e-09</v>
+        <v>0.000135804</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>4.307246446609497</v>
+        <v>4.304245948791504</v>
       </c>
       <c r="B50" t="n">
-        <v>9.479139e-09</v>
+        <v>0.0001358122</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>4.409252405166626</v>
+        <v>4.405251741409302</v>
       </c>
       <c r="B51" t="n">
-        <v>9.425500999999999e-09</v>
+        <v>0.0001357843</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>4.502257585525513</v>
+        <v>4.5062575340271</v>
       </c>
       <c r="B52" t="n">
-        <v>9.504139e-09</v>
+        <v>0.000135601</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>4.603263378143311</v>
+        <v>4.604263067245483</v>
       </c>
       <c r="B53" t="n">
-        <v>9.314174000000001e-09</v>
+        <v>0.0001357511</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>4.703269243240356</v>
+        <v>4.707268953323364</v>
       </c>
       <c r="B54" t="n">
-        <v>9.428993000000001e-09</v>
+        <v>0.0001357542</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>4.802274942398071</v>
+        <v>4.807274580001831</v>
       </c>
       <c r="B55" t="n">
-        <v>9.475091e-09</v>
+        <v>0.0001356641</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>4.900280475616455</v>
+        <v>4.907280445098877</v>
       </c>
       <c r="B56" t="n">
-        <v>9.261496e-09</v>
+        <v>0.0001356808</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>5.000286102294922</v>
+        <v>5.007286071777344</v>
       </c>
       <c r="B57" t="n">
-        <v>9.446086e-09</v>
+        <v>0.0001356616</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>5.109292268753052</v>
+        <v>5.108292102813721</v>
       </c>
       <c r="B58" t="n">
-        <v>9.334912000000001e-09</v>
+        <v>0.0001356345</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>5.209298133850098</v>
+        <v>5.204297304153442</v>
       </c>
       <c r="B59" t="n">
-        <v>9.348511e-09</v>
+        <v>0.0001356351</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>5.309303998947144</v>
+        <v>5.304303169250488</v>
       </c>
       <c r="B60" t="n">
-        <v>9.288891e-09</v>
+        <v>0.0001356867</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>5.40930962562561</v>
+        <v>5.406309127807617</v>
       </c>
       <c r="B61" t="n">
-        <v>9.351818e-09</v>
+        <v>0.0001356805</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>5.509315252304077</v>
+        <v>5.500314235687256</v>
       </c>
       <c r="B62" t="n">
-        <v>9.322555000000001e-09</v>
+        <v>0.0001356669</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>5.609321117401123</v>
+        <v>5.607320547103882</v>
       </c>
       <c r="B63" t="n">
-        <v>9.390326e-09</v>
+        <v>0.0001357159</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>5.700326204299927</v>
+        <v>5.709326505661011</v>
       </c>
       <c r="B64" t="n">
-        <v>9.306519999999999e-09</v>
+        <v>0.0001357218</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>5.800331830978394</v>
+        <v>5.806331872940063</v>
       </c>
       <c r="B65" t="n">
-        <v>9.251121e-09</v>
+        <v>0.0001357276</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>5.90033745765686</v>
+        <v>5.914337873458862</v>
       </c>
       <c r="B66" t="n">
-        <v>9.289675e-09</v>
+        <v>0.0001356562</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>6.000343322753906</v>
+        <v>6.017343997955322</v>
       </c>
       <c r="B67" t="n">
-        <v>9.28866e-09</v>
+        <v>0.0001357369</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>6.102349042892456</v>
+        <v>6.113349437713623</v>
       </c>
       <c r="B68" t="n">
-        <v>9.449669999999999e-09</v>
+        <v>0.000135717</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>6.204355001449585</v>
+        <v>6.21435546875</v>
       </c>
       <c r="B69" t="n">
-        <v>9.352449999999999e-09</v>
+        <v>0.0001357607</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>6.305360794067383</v>
+        <v>6.318361282348633</v>
       </c>
       <c r="B70" t="n">
-        <v>9.41952e-09</v>
+        <v>0.0001357345</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>6.406366586685181</v>
+        <v>6.423367023468018</v>
       </c>
       <c r="B71" t="n">
-        <v>9.353304e-09</v>
+        <v>0.0001358011</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>6.506372451782227</v>
+        <v>6.527373313903809</v>
       </c>
       <c r="B72" t="n">
-        <v>9.344687e-09</v>
+        <v>0.000135863</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>6.607378005981445</v>
+        <v>6.633379220962524</v>
       </c>
       <c r="B73" t="n">
-        <v>9.409723000000001e-09</v>
+        <v>0.0001358288</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>6.708383798599243</v>
+        <v>6.737385034561157</v>
       </c>
       <c r="B74" t="n">
-        <v>9.457305e-09</v>
+        <v>0.0001358048</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>6.809389591217041</v>
+        <v>6.844391345977783</v>
       </c>
       <c r="B75" t="n">
-        <v>9.259389e-09</v>
+        <v>0.0001358959</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>6.900394916534424</v>
+        <v>6.951397180557251</v>
       </c>
       <c r="B76" t="n">
-        <v>9.359393999999999e-09</v>
+        <v>0.0001358679</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>7.001400709152222</v>
+        <v>7.046402931213379</v>
       </c>
       <c r="B77" t="n">
-        <v>9.357085e-09</v>
+        <v>0.0001358107</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>7.10240650177002</v>
+        <v>7.147408723831177</v>
       </c>
       <c r="B78" t="n">
-        <v>9.241740999999999e-09</v>
+        <v>0.0001358484</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>7.2054123878479</v>
+        <v>7.2314133644104</v>
       </c>
       <c r="B79" t="n">
-        <v>9.494992999999999e-09</v>
+        <v>0.0001357897</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>7.306417942047119</v>
+        <v>7.32741904258728</v>
       </c>
       <c r="B80" t="n">
-        <v>9.405566000000001e-09</v>
+        <v>0.0001358554</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>7.408424139022827</v>
+        <v>7.420424461364746</v>
       </c>
       <c r="B81" t="n">
-        <v>9.228879000000001e-09</v>
+        <v>0.0001358428</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>7.500429153442383</v>
+        <v>7.500428676605225</v>
       </c>
       <c r="B82" t="n">
-        <v>9.285831e-09</v>
+        <v>0.0001358464</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>7.602434873580933</v>
+        <v>7.600434541702271</v>
       </c>
       <c r="B83" t="n">
-        <v>9.438688000000001e-09</v>
+        <v>0.000135774</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>7.70344066619873</v>
+        <v>7.708440780639648</v>
       </c>
       <c r="B84" t="n">
-        <v>9.254703e-09</v>
+        <v>0.0001357856</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>7.805446863174438</v>
+        <v>7.804446220397949</v>
       </c>
       <c r="B85" t="n">
-        <v>9.511266e-09</v>
+        <v>0.0001358506</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>7.907452583312988</v>
+        <v>7.923453092575073</v>
       </c>
       <c r="B86" t="n">
-        <v>9.347019e-09</v>
+        <v>0.0001357727</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>8.008458375930786</v>
+        <v>8.033459424972534</v>
       </c>
       <c r="B87" t="n">
-        <v>9.428611e-09</v>
+        <v>0.0001357942</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>8.100463390350342</v>
+        <v>8.138465166091919</v>
       </c>
       <c r="B88" t="n">
-        <v>9.243107e-09</v>
+        <v>0.0001358025</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>8.203469514846802</v>
+        <v>8.20746922492981</v>
       </c>
       <c r="B89" t="n">
-        <v>9.236087e-09</v>
+        <v>0.0001357973</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>8.306475162506104</v>
+        <v>8.301474809646606</v>
       </c>
       <c r="B90" t="n">
-        <v>9.222568000000001e-09</v>
+        <v>0.0001358451</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>8.408481121063232</v>
+        <v>8.400480270385742</v>
       </c>
       <c r="B91" t="n">
-        <v>9.351540999999999e-09</v>
+        <v>0.0001358078</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>8.500486135482788</v>
+        <v>8.503486156463623</v>
       </c>
       <c r="B92" t="n">
-        <v>9.2078e-09</v>
+        <v>0.0001358293</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>8.602492332458496</v>
+        <v>8.605492115020752</v>
       </c>
       <c r="B93" t="n">
-        <v>9.331038e-09</v>
+        <v>0.0001358156</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>8.705498218536377</v>
+        <v>8.709497928619385</v>
       </c>
       <c r="B94" t="n">
-        <v>9.350626e-09</v>
+        <v>0.0001358386</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>8.807503938674927</v>
+        <v>8.807503461837769</v>
       </c>
       <c r="B95" t="n">
-        <v>9.449698e-09</v>
+        <v>0.0001358952</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>8.909509658813477</v>
+        <v>8.906509160995483</v>
       </c>
       <c r="B96" t="n">
-        <v>9.369444e-09</v>
+        <v>0.0001358972</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>9.00151515007019</v>
+        <v>9.009515285491943</v>
       </c>
       <c r="B97" t="n">
-        <v>9.426808000000001e-09</v>
+        <v>0.0001358467</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>9.101520776748657</v>
+        <v>9.106520652770996</v>
       </c>
       <c r="B98" t="n">
-        <v>9.417357999999999e-09</v>
+        <v>0.0001358869</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>9.201526403427124</v>
+        <v>9.213526725769043</v>
       </c>
       <c r="B99" t="n">
-        <v>9.480377000000001e-09</v>
+        <v>0.0001358369</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>9.301532030105591</v>
+        <v>9.316532611846924</v>
       </c>
       <c r="B100" t="n">
-        <v>9.426468e-09</v>
+        <v>0.0001358947</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>9.402537822723389</v>
+        <v>9.40953803062439</v>
       </c>
       <c r="B101" t="n">
-        <v>9.550184e-09</v>
+        <v>0.0001358204</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>9.502543687820435</v>
+        <v>9.502543210983276</v>
       </c>
       <c r="B102" t="n">
-        <v>9.545281999999999e-09</v>
+        <v>0.0001358759</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>9.601549386978149</v>
+        <v>9.609549522399902</v>
       </c>
       <c r="B103" t="n">
-        <v>9.511697e-09</v>
+        <v>0.0001358819</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>9.702555179595947</v>
+        <v>9.706555128097534</v>
       </c>
       <c r="B104" t="n">
-        <v>9.523930000000001e-09</v>
+        <v>0.0001358695</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>9.802560806274414</v>
+        <v>9.804560661315918</v>
       </c>
       <c r="B105" t="n">
-        <v>9.545581e-09</v>
+        <v>0.0001357965</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>9.902566432952881</v>
+        <v>9.901566028594971</v>
       </c>
       <c r="B106" t="n">
-        <v>9.458604e-09</v>
+        <v>0.0001357987</v>
       </c>
     </row>
     <row r="107">
@@ -1281,2175 +1281,2175 @@
         <v>10.00257205963135</v>
       </c>
       <c r="B107" t="n">
-        <v>9.517634e-09</v>
+        <v>0.0001358362</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>10.10357785224915</v>
+        <v>10.10957813262939</v>
       </c>
       <c r="B108" t="n">
-        <v>9.278475e-09</v>
+        <v>0.0001358162</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>10.20358395576477</v>
+        <v>10.20358347892761</v>
       </c>
       <c r="B109" t="n">
-        <v>9.371655e-09</v>
+        <v>0.0001357525</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>10.30458950996399</v>
+        <v>10.30858945846558</v>
       </c>
       <c r="B110" t="n">
-        <v>9.444741e-09</v>
+        <v>0.0001357994</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>10.40559530258179</v>
+        <v>10.40759515762329</v>
       </c>
       <c r="B111" t="n">
-        <v>9.513877000000001e-09</v>
+        <v>0.0001357483</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>10.50660109519958</v>
+        <v>10.50160050392151</v>
       </c>
       <c r="B112" t="n">
-        <v>9.247225000000001e-09</v>
+        <v>0.0001357964</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>10.60660696029663</v>
+        <v>10.60260629653931</v>
       </c>
       <c r="B113" t="n">
-        <v>9.328822e-09</v>
+        <v>0.0001358038</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>10.70761251449585</v>
+        <v>10.70561218261719</v>
       </c>
       <c r="B114" t="n">
-        <v>9.392273e-09</v>
+        <v>0.0001357656</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>10.8076183795929</v>
+        <v>10.80861806869507</v>
       </c>
       <c r="B115" t="n">
-        <v>9.446607999999999e-09</v>
+        <v>0.0001357134</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>10.90762400627136</v>
+        <v>10.90862369537354</v>
       </c>
       <c r="B116" t="n">
-        <v>9.485221e-09</v>
+        <v>0.0001357612</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>11.00862979888916</v>
+        <v>11.00762939453125</v>
       </c>
       <c r="B117" t="n">
-        <v>9.440867999999999e-09</v>
+        <v>0.0001357274</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>11.10863542556763</v>
+        <v>11.10463500022888</v>
       </c>
       <c r="B118" t="n">
-        <v>9.262520999999999e-09</v>
+        <v>0.0001357061</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>11.20964121818542</v>
+        <v>11.20764088630676</v>
       </c>
       <c r="B119" t="n">
-        <v>9.446839e-09</v>
+        <v>0.0001357254</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>11.30064654350281</v>
+        <v>11.30564641952515</v>
       </c>
       <c r="B120" t="n">
-        <v>9.287875e-09</v>
+        <v>0.0001357553</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>11.40065217018127</v>
+        <v>11.40465211868286</v>
       </c>
       <c r="B121" t="n">
-        <v>9.264605e-09</v>
+        <v>0.0001357309</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>11.50065803527832</v>
+        <v>11.50065755844116</v>
       </c>
       <c r="B122" t="n">
-        <v>9.407585000000001e-09</v>
+        <v>0.0001357802</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>11.60166382789612</v>
+        <v>11.60766386985779</v>
       </c>
       <c r="B123" t="n">
-        <v>9.467998e-09</v>
+        <v>0.000135729</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>11.70166945457458</v>
+        <v>11.70766949653625</v>
       </c>
       <c r="B124" t="n">
-        <v>9.504775000000001e-09</v>
+        <v>0.0001357612</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>11.80267524719238</v>
+        <v>11.80367493629456</v>
       </c>
       <c r="B125" t="n">
-        <v>9.406468e-09</v>
+        <v>0.0001357232</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>11.90368103981018</v>
+        <v>11.90468096733093</v>
       </c>
       <c r="B126" t="n">
-        <v>9.34806e-09</v>
+        <v>0.0001357185</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>12.00468683242798</v>
+        <v>12.00668668746948</v>
       </c>
       <c r="B127" t="n">
-        <v>9.393159e-09</v>
+        <v>0.0001357023</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>12.10569262504578</v>
+        <v>12.10169196128845</v>
       </c>
       <c r="B128" t="n">
-        <v>9.203081999999999e-09</v>
+        <v>0.0001357211</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>12.20669841766357</v>
+        <v>12.20969820022583</v>
       </c>
       <c r="B129" t="n">
-        <v>9.313548e-09</v>
+        <v>0.0001357022</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>12.30870413780212</v>
+        <v>12.30770373344421</v>
       </c>
       <c r="B130" t="n">
-        <v>9.267535e-09</v>
+        <v>0.000135683</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>12.40970993041992</v>
+        <v>12.40970945358276</v>
       </c>
       <c r="B131" t="n">
-        <v>9.268666e-09</v>
+        <v>0.0001356514</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>12.50171518325806</v>
+        <v>12.5197160243988</v>
       </c>
       <c r="B132" t="n">
-        <v>9.363631e-09</v>
+        <v>0.0001356277</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>12.60272121429443</v>
+        <v>12.60072064399719</v>
       </c>
       <c r="B133" t="n">
-        <v>9.211846999999999e-09</v>
+        <v>0.0001356508</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>12.70472693443298</v>
+        <v>12.70872664451599</v>
       </c>
       <c r="B134" t="n">
-        <v>9.399198999999999e-09</v>
+        <v>0.0001355486</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>12.80573272705078</v>
+        <v>12.80273222923279</v>
       </c>
       <c r="B135" t="n">
-        <v>9.167473999999999e-09</v>
+        <v>0.0001355789</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>12.90873837471008</v>
+        <v>12.90673804283142</v>
       </c>
       <c r="B136" t="n">
-        <v>9.321045999999999e-09</v>
+        <v>0.0001354293</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>13.0007438659668</v>
+        <v>13.00874376296997</v>
       </c>
       <c r="B137" t="n">
-        <v>9.261040000000001e-09</v>
+        <v>0.0001353725</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>13.10274958610535</v>
+        <v>13.10774946212769</v>
       </c>
       <c r="B138" t="n">
-        <v>9.220835000000001e-09</v>
+        <v>0.000135279</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>13.20575547218323</v>
+        <v>13.21775579452515</v>
       </c>
       <c r="B139" t="n">
-        <v>9.376550000000001e-09</v>
+        <v>0.0001351942</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>13.30776119232178</v>
+        <v>13.31676149368286</v>
       </c>
       <c r="B140" t="n">
-        <v>9.464738e-09</v>
+        <v>0.0001351015</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>13.40976691246033</v>
+        <v>13.40876698493958</v>
       </c>
       <c r="B141" t="n">
-        <v>9.350391e-09</v>
+        <v>0.0001350895</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>13.50177240371704</v>
+        <v>13.51677298545837</v>
       </c>
       <c r="B142" t="n">
-        <v>9.480235e-09</v>
+        <v>0.0001349918</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>13.60377812385559</v>
+        <v>13.60877823829651</v>
       </c>
       <c r="B143" t="n">
-        <v>9.350539999999999e-09</v>
+        <v>0.0001348671</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>13.70678400993347</v>
+        <v>13.7017834186554</v>
       </c>
       <c r="B144" t="n">
-        <v>9.276989000000001e-09</v>
+        <v>0.0001347714</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>13.8087899684906</v>
+        <v>13.8107898235321</v>
       </c>
       <c r="B145" t="n">
-        <v>9.14484e-09</v>
+        <v>0.0001346452</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>13.90179538726807</v>
+        <v>13.9047954082489</v>
       </c>
       <c r="B146" t="n">
-        <v>9.506669999999999e-09</v>
+        <v>0.0001346259</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>14.0058012008667</v>
+        <v>14.00080060958862</v>
       </c>
       <c r="B147" t="n">
-        <v>9.280710000000001e-09</v>
+        <v>0.0001345069</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>14.10980725288391</v>
+        <v>14.10680675506592</v>
       </c>
       <c r="B148" t="n">
-        <v>9.332120999999999e-09</v>
+        <v>0.0001343379</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>14.20381236076355</v>
+        <v>14.20581245422363</v>
       </c>
       <c r="B149" t="n">
-        <v>9.337797e-09</v>
+        <v>0.000134182</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>14.30781865119934</v>
+        <v>14.30681800842285</v>
       </c>
       <c r="B150" t="n">
-        <v>9.414765e-09</v>
+        <v>0.0001339679</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>14.40182375907898</v>
+        <v>14.40982389450073</v>
       </c>
       <c r="B151" t="n">
-        <v>9.421861e-09</v>
+        <v>0.0001339344</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>14.50482988357544</v>
+        <v>14.50382947921753</v>
       </c>
       <c r="B152" t="n">
-        <v>9.439264000000001e-09</v>
+        <v>0.0001338004</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>14.60783576965332</v>
+        <v>14.60883545875549</v>
       </c>
       <c r="B153" t="n">
-        <v>9.277928000000001e-09</v>
+        <v>0.0001336452</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>14.70184087753296</v>
+        <v>14.70284080505371</v>
       </c>
       <c r="B154" t="n">
-        <v>9.427876e-09</v>
+        <v>0.0001334778</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>14.80584716796875</v>
+        <v>14.80684661865234</v>
       </c>
       <c r="B155" t="n">
-        <v>9.186532e-09</v>
+        <v>0.0001334595</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>14.90985298156738</v>
+        <v>14.90885257720947</v>
       </c>
       <c r="B156" t="n">
-        <v>9.392436000000001e-09</v>
+        <v>0.000133417</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>15.0038583278656</v>
+        <v>15.00285792350769</v>
       </c>
       <c r="B157" t="n">
-        <v>9.362553999999999e-09</v>
+        <v>0.0001333448</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>15.10886430740356</v>
+        <v>15.10786390304565</v>
       </c>
       <c r="B158" t="n">
-        <v>9.120484e-09</v>
+        <v>0.0001333526</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>15.20286965370178</v>
+        <v>15.20486950874329</v>
       </c>
       <c r="B159" t="n">
-        <v>9.34053e-09</v>
+        <v>0.0001334148</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>15.30687570571899</v>
+        <v>15.30087494850159</v>
       </c>
       <c r="B160" t="n">
-        <v>9.30555e-09</v>
+        <v>0.0001334244</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>15.40088105201721</v>
+        <v>15.4048810005188</v>
       </c>
       <c r="B161" t="n">
-        <v>9.281603999999999e-09</v>
+        <v>0.0001335476</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>15.50388693809509</v>
+        <v>15.5078866481781</v>
       </c>
       <c r="B162" t="n">
-        <v>9.28245e-09</v>
+        <v>0.0001336375</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>15.60789275169373</v>
+        <v>15.60289216041565</v>
       </c>
       <c r="B163" t="n">
-        <v>9.383882e-09</v>
+        <v>0.0001336487</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>15.70189833641052</v>
+        <v>15.70589804649353</v>
       </c>
       <c r="B164" t="n">
-        <v>9.43276e-09</v>
+        <v>0.0001339259</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>15.80890417098999</v>
+        <v>15.80990409851074</v>
       </c>
       <c r="B165" t="n">
-        <v>9.231929e-09</v>
+        <v>0.0001340076</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>15.90190982818604</v>
+        <v>15.90390944480896</v>
       </c>
       <c r="B166" t="n">
-        <v>9.427280999999999e-09</v>
+        <v>0.0001341342</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>16.00591564178467</v>
+        <v>16.00891542434692</v>
       </c>
       <c r="B167" t="n">
-        <v>9.20391e-09</v>
+        <v>0.0001343473</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>16.10092091560364</v>
+        <v>16.10392069816589</v>
       </c>
       <c r="B168" t="n">
-        <v>9.228276e-09</v>
+        <v>0.0001344578</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>16.20392680168152</v>
+        <v>16.20792698860168</v>
       </c>
       <c r="B169" t="n">
-        <v>9.390897e-09</v>
+        <v>0.0001345402</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>16.30993318557739</v>
+        <v>16.30293250083923</v>
       </c>
       <c r="B170" t="n">
-        <v>9.244630999999999e-09</v>
+        <v>0.0001346756</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>16.40393829345703</v>
+        <v>16.40793824195862</v>
       </c>
       <c r="B171" t="n">
-        <v>9.295158999999999e-09</v>
+        <v>0.0001347423</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>16.50994443893433</v>
+        <v>16.5109441280365</v>
       </c>
       <c r="B172" t="n">
-        <v>9.440364999999999e-09</v>
+        <v>0.0001348389</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>16.60094952583313</v>
+        <v>16.61295008659363</v>
       </c>
       <c r="B173" t="n">
-        <v>9.227083e-09</v>
+        <v>0.0001349228</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>16.70995593070984</v>
+        <v>16.70395541191101</v>
       </c>
       <c r="B174" t="n">
-        <v>9.400662000000001e-09</v>
+        <v>0.0001349367</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>16.80996155738831</v>
+        <v>16.80596113204956</v>
       </c>
       <c r="B175" t="n">
-        <v>9.476184000000001e-09</v>
+        <v>0.000135003</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>16.9039671421051</v>
+        <v>16.90396666526794</v>
       </c>
       <c r="B176" t="n">
-        <v>9.274824e-09</v>
+        <v>0.0001350099</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>17.00797295570374</v>
+        <v>17.00797247886658</v>
       </c>
       <c r="B177" t="n">
-        <v>9.364114e-09</v>
+        <v>0.0001349895</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>17.10197830200195</v>
+        <v>17.10697817802429</v>
       </c>
       <c r="B178" t="n">
-        <v>9.436915e-09</v>
+        <v>0.00013499</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>17.20998454093933</v>
+        <v>17.20698404312134</v>
       </c>
       <c r="B179" t="n">
-        <v>9.490153e-09</v>
+        <v>0.0001349604</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>17.30499005317688</v>
+        <v>17.30298948287964</v>
       </c>
       <c r="B180" t="n">
-        <v>9.412514e-09</v>
+        <v>0.0001349458</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>17.40099549293518</v>
+        <v>17.40499544143677</v>
       </c>
       <c r="B181" t="n">
-        <v>9.302995000000001e-09</v>
+        <v>0.000134944</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>17.50600147247314</v>
+        <v>17.50100088119507</v>
       </c>
       <c r="B182" t="n">
-        <v>9.1692e-09</v>
+        <v>0.0001348736</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>17.60200691223145</v>
+        <v>17.60700678825378</v>
       </c>
       <c r="B183" t="n">
-        <v>9.388116e-09</v>
+        <v>0.0001348673</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>17.70601296424866</v>
+        <v>17.70301222801208</v>
       </c>
       <c r="B184" t="n">
-        <v>9.142036e-09</v>
+        <v>0.0001348567</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>17.80001831054688</v>
+        <v>17.81201863288879</v>
       </c>
       <c r="B185" t="n">
-        <v>9.189613999999999e-09</v>
+        <v>0.0001348224</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>17.90502429008484</v>
+        <v>17.90802407264709</v>
       </c>
       <c r="B186" t="n">
-        <v>9.361944e-09</v>
+        <v>0.0001348843</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>18.00202989578247</v>
+        <v>18.00802993774414</v>
       </c>
       <c r="B187" t="n">
-        <v>9.398517e-09</v>
+        <v>0.0001348632</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>18.10903596878052</v>
+        <v>18.10403513908386</v>
       </c>
       <c r="B188" t="n">
-        <v>9.161817000000001e-09</v>
+        <v>0.0001348289</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>18.20304131507874</v>
+        <v>18.20704126358032</v>
       </c>
       <c r="B189" t="n">
-        <v>9.210876000000001e-09</v>
+        <v>0.0001348088</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>18.30704736709595</v>
+        <v>18.30204653739929</v>
       </c>
       <c r="B190" t="n">
-        <v>9.275321e-09</v>
+        <v>0.0001348898</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>18.40205264091492</v>
+        <v>18.40805268287659</v>
       </c>
       <c r="B191" t="n">
-        <v>9.358466e-09</v>
+        <v>0.0001348809</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>18.50605869293213</v>
+        <v>18.50205826759338</v>
       </c>
       <c r="B192" t="n">
-        <v>9.090509000000001e-09</v>
+        <v>0.0001348445</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>18.60906457901001</v>
+        <v>18.6080641746521</v>
       </c>
       <c r="B193" t="n">
-        <v>9.282308999999999e-09</v>
+        <v>0.0001349125</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>18.70106983184814</v>
+        <v>18.70206952095032</v>
       </c>
       <c r="B194" t="n">
-        <v>9.171028999999999e-09</v>
+        <v>0.0001349525</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>18.80207538604736</v>
+        <v>18.80407547950745</v>
       </c>
       <c r="B195" t="n">
-        <v>9.412079999999999e-09</v>
+        <v>0.0001349475</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>18.90408158302307</v>
+        <v>18.906081199646</v>
       </c>
       <c r="B196" t="n">
-        <v>9.132146000000001e-09</v>
+        <v>0.0001349353</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>19.00508737564087</v>
+        <v>19.00908708572388</v>
       </c>
       <c r="B197" t="n">
-        <v>9.337308e-09</v>
+        <v>0.0001349964</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>19.10709309577942</v>
+        <v>19.10009241104126</v>
       </c>
       <c r="B198" t="n">
-        <v>9.297452999999999e-09</v>
+        <v>0.0001349822</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>19.20909881591797</v>
+        <v>19.20609831809998</v>
       </c>
       <c r="B199" t="n">
-        <v>9.185102e-09</v>
+        <v>0.0001349886</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>19.30010414123535</v>
+        <v>19.30310392379761</v>
       </c>
       <c r="B200" t="n">
-        <v>9.375214e-09</v>
+        <v>0.0001350304</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>19.40211009979248</v>
+        <v>19.40910983085632</v>
       </c>
       <c r="B201" t="n">
-        <v>9.3606e-09</v>
+        <v>0.0001349822</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>19.50411581993103</v>
+        <v>19.5051155090332</v>
       </c>
       <c r="B202" t="n">
-        <v>9.261907000000001e-09</v>
+        <v>0.0001350289</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>19.60712146759033</v>
+        <v>19.60312104225159</v>
       </c>
       <c r="B203" t="n">
-        <v>9.267133999999999e-09</v>
+        <v>0.0001349873</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>19.70912742614746</v>
+        <v>19.70512676239014</v>
       </c>
       <c r="B204" t="n">
-        <v>9.327438e-09</v>
+        <v>0.0001350228</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>19.80013275146484</v>
+        <v>19.80913305282593</v>
       </c>
       <c r="B205" t="n">
-        <v>9.324828999999999e-09</v>
+        <v>0.0001349536</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>19.90213847160339</v>
+        <v>19.90313816070557</v>
       </c>
       <c r="B206" t="n">
-        <v>9.321541e-09</v>
+        <v>0.0001348847</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>20.00314426422119</v>
+        <v>20.00314402580261</v>
       </c>
       <c r="B207" t="n">
-        <v>9.098224e-09</v>
+        <v>0.0001348105</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>20.10615015029907</v>
+        <v>20.10815000534058</v>
       </c>
       <c r="B208" t="n">
-        <v>9.139641000000001e-09</v>
+        <v>0.000134782</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>20.20915603637695</v>
+        <v>20.20115518569946</v>
       </c>
       <c r="B209" t="n">
-        <v>9.303853e-09</v>
+        <v>0.0001347328</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>20.3041615486145</v>
+        <v>20.30616140365601</v>
       </c>
       <c r="B210" t="n">
-        <v>9.220655e-09</v>
+        <v>0.0001346308</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>20.40816760063171</v>
+        <v>20.40116667747498</v>
       </c>
       <c r="B211" t="n">
-        <v>9.470387999999999e-09</v>
+        <v>0.0001345037</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>20.5011727809906</v>
+        <v>20.5031726360321</v>
       </c>
       <c r="B212" t="n">
-        <v>9.329504999999999e-09</v>
+        <v>0.0001344351</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>20.60517883300781</v>
+        <v>20.60817861557007</v>
       </c>
       <c r="B213" t="n">
-        <v>9.390625999999999e-09</v>
+        <v>0.0001343149</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>20.70718455314636</v>
+        <v>20.70218396186829</v>
       </c>
       <c r="B214" t="n">
-        <v>9.442549999999999e-09</v>
+        <v>0.0001343105</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>20.80018973350525</v>
+        <v>20.80418992042542</v>
       </c>
       <c r="B215" t="n">
-        <v>9.168361999999999e-09</v>
+        <v>0.0001341874</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>20.90419602394104</v>
+        <v>20.90719556808472</v>
       </c>
       <c r="B216" t="n">
-        <v>9.224986e-09</v>
+        <v>0.0001340363</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>21.00620174407959</v>
+        <v>21.00020098686218</v>
       </c>
       <c r="B217" t="n">
-        <v>9.342497e-09</v>
+        <v>0.0001341025</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>21.10020685195923</v>
+        <v>21.10220694541931</v>
       </c>
       <c r="B218" t="n">
-        <v>9.352116999999999e-09</v>
+        <v>0.0001340261</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>21.20321297645569</v>
+        <v>21.2072126865387</v>
       </c>
       <c r="B219" t="n">
-        <v>9.256084000000001e-09</v>
+        <v>0.0001340784</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>21.30521869659424</v>
+        <v>21.30021810531616</v>
       </c>
       <c r="B220" t="n">
-        <v>9.395038e-09</v>
+        <v>0.0001341196</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>21.40822458267212</v>
+        <v>21.40222406387329</v>
       </c>
       <c r="B221" t="n">
-        <v>9.483796e-09</v>
+        <v>0.0001342153</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>21.50023007392883</v>
+        <v>21.50522994995117</v>
       </c>
       <c r="B222" t="n">
-        <v>9.231479999999999e-09</v>
+        <v>0.0001341426</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>21.60323596000671</v>
+        <v>21.60823559761047</v>
       </c>
       <c r="B223" t="n">
-        <v>9.163917e-09</v>
+        <v>0.0001342133</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>21.70624160766602</v>
+        <v>21.70024108886719</v>
       </c>
       <c r="B224" t="n">
-        <v>9.271564e-09</v>
+        <v>0.0001343588</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>21.80824756622314</v>
+        <v>21.80124688148499</v>
       </c>
       <c r="B225" t="n">
-        <v>9.218484000000001e-09</v>
+        <v>0.0001344747</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>21.90125274658203</v>
+        <v>21.90625262260437</v>
       </c>
       <c r="B226" t="n">
-        <v>9.166243999999999e-09</v>
+        <v>0.0001346137</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>22.00425863265991</v>
+        <v>22.00025820732117</v>
       </c>
       <c r="B227" t="n">
-        <v>9.20407e-09</v>
+        <v>0.000134694</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>22.10626435279846</v>
+        <v>22.1042640209198</v>
       </c>
       <c r="B228" t="n">
-        <v>9.316605e-09</v>
+        <v>0.0001347231</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>22.20927047729492</v>
+        <v>22.20927023887634</v>
       </c>
       <c r="B229" t="n">
-        <v>9.378023e-09</v>
+        <v>0.0001348361</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>22.30327582359314</v>
+        <v>22.30227541923523</v>
       </c>
       <c r="B230" t="n">
-        <v>9.121765e-09</v>
+        <v>0.0001348747</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>22.40628170967102</v>
+        <v>22.40428113937378</v>
       </c>
       <c r="B231" t="n">
-        <v>9.238688000000001e-09</v>
+        <v>0.0001349197</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>22.5092875957489</v>
+        <v>22.50728726387024</v>
       </c>
       <c r="B232" t="n">
-        <v>9.185856999999999e-09</v>
+        <v>0.0001350019</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>22.60929346084595</v>
+        <v>22.60329270362854</v>
       </c>
       <c r="B233" t="n">
-        <v>9.215012000000001e-09</v>
+        <v>0.0001350748</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>22.70929908752441</v>
+        <v>22.70429849624634</v>
       </c>
       <c r="B234" t="n">
-        <v>9.151367e-09</v>
+        <v>0.0001351022</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>22.80830478668213</v>
+        <v>22.80430436134338</v>
       </c>
       <c r="B235" t="n">
-        <v>9.421932e-09</v>
+        <v>0.0001351202</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>22.90731048583984</v>
+        <v>22.90330982208252</v>
       </c>
       <c r="B236" t="n">
-        <v>9.366609e-09</v>
+        <v>0.0001352099</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>23.00631618499756</v>
+        <v>23.00331568717957</v>
       </c>
       <c r="B237" t="n">
-        <v>9.251855999999999e-09</v>
+        <v>0.0001352618</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>23.10732197761536</v>
+        <v>23.10532140731812</v>
       </c>
       <c r="B238" t="n">
-        <v>9.313212e-09</v>
+        <v>0.0001352544</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>23.20732760429382</v>
+        <v>23.20432710647583</v>
       </c>
       <c r="B239" t="n">
-        <v>9.353278e-09</v>
+        <v>0.0001352012</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>23.30733323097229</v>
+        <v>23.3043327331543</v>
       </c>
       <c r="B240" t="n">
-        <v>9.322638999999999e-09</v>
+        <v>0.0001352384</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>23.40633893013</v>
+        <v>23.40733861923218</v>
       </c>
       <c r="B241" t="n">
-        <v>9.280743e-09</v>
+        <v>0.0001352351</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>23.50634455680847</v>
+        <v>23.50734424591064</v>
       </c>
       <c r="B242" t="n">
-        <v>9.226888e-09</v>
+        <v>0.0001352463</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>23.60635042190552</v>
+        <v>23.61635065078735</v>
       </c>
       <c r="B243" t="n">
-        <v>9.201515e-09</v>
+        <v>0.0001352545</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>23.70535612106323</v>
+        <v>23.70635581016541</v>
       </c>
       <c r="B244" t="n">
-        <v>9.438416e-09</v>
+        <v>0.0001352465</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>23.8053617477417</v>
+        <v>23.80636143684387</v>
       </c>
       <c r="B245" t="n">
-        <v>9.311501999999999e-09</v>
+        <v>0.0001351602</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>23.90536737442017</v>
+        <v>23.90636706352234</v>
       </c>
       <c r="B246" t="n">
-        <v>9.428172e-09</v>
+        <v>0.0001351664</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>24.00537323951721</v>
+        <v>24.00837302207947</v>
       </c>
       <c r="B247" t="n">
-        <v>9.437501e-09</v>
+        <v>0.0001352088</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>24.10537886619568</v>
+        <v>24.10337853431702</v>
       </c>
       <c r="B248" t="n">
-        <v>9.429977e-09</v>
+        <v>0.0001351668</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>24.20538449287415</v>
+        <v>24.20238399505615</v>
       </c>
       <c r="B249" t="n">
-        <v>9.452555999999999e-09</v>
+        <v>0.0001351616</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>24.30539035797119</v>
+        <v>24.30338978767395</v>
       </c>
       <c r="B250" t="n">
-        <v>9.418431e-09</v>
+        <v>0.0001351525</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>24.40539598464966</v>
+        <v>24.40239548683167</v>
       </c>
       <c r="B251" t="n">
-        <v>9.427794000000001e-09</v>
+        <v>0.0001351414</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>24.5054018497467</v>
+        <v>24.50140118598938</v>
       </c>
       <c r="B252" t="n">
-        <v>9.149584000000001e-09</v>
+        <v>0.0001350526</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>24.60540747642517</v>
+        <v>24.60040688514709</v>
       </c>
       <c r="B253" t="n">
-        <v>9.240487e-09</v>
+        <v>0.0001351064</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>24.70641350746155</v>
+        <v>24.70141267776489</v>
       </c>
       <c r="B254" t="n">
-        <v>9.145128e-09</v>
+        <v>0.0001350197</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>24.80641913414001</v>
+        <v>24.80141830444336</v>
       </c>
       <c r="B255" t="n">
-        <v>9.160301000000001e-09</v>
+        <v>0.0001350205</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>24.90542483329773</v>
+        <v>24.90142393112183</v>
       </c>
       <c r="B256" t="n">
-        <v>9.292807000000001e-09</v>
+        <v>0.0001350429</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>25.0054304599762</v>
+        <v>25.00042963027954</v>
       </c>
       <c r="B257" t="n">
-        <v>9.367527e-09</v>
+        <v>0.0001350159</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>25.10643625259399</v>
+        <v>25.10943603515625</v>
       </c>
       <c r="B258" t="n">
-        <v>9.210334e-09</v>
+        <v>0.0001350099</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>25.20944213867188</v>
+        <v>25.20144128799438</v>
       </c>
       <c r="B259" t="n">
-        <v>9.293409000000001e-09</v>
+        <v>0.0001350096</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>25.30944776535034</v>
+        <v>25.30344724655151</v>
       </c>
       <c r="B260" t="n">
-        <v>9.290336e-09</v>
+        <v>0.0001349214</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>25.40945339202881</v>
+        <v>25.40345287322998</v>
       </c>
       <c r="B261" t="n">
-        <v>9.334828e-09</v>
+        <v>0.0001349186</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>25.50045895576477</v>
+        <v>25.50345849990845</v>
       </c>
       <c r="B262" t="n">
-        <v>9.268810000000001e-09</v>
+        <v>0.0001349035</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>25.60146450996399</v>
+        <v>25.60346436500549</v>
       </c>
       <c r="B263" t="n">
-        <v>9.369604e-09</v>
+        <v>0.0001348748</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>25.70247030258179</v>
+        <v>25.70447015762329</v>
       </c>
       <c r="B264" t="n">
-        <v>9.429118999999999e-09</v>
+        <v>0.0001348443</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>25.80247592926025</v>
+        <v>25.80547571182251</v>
       </c>
       <c r="B265" t="n">
-        <v>9.360372e-09</v>
+        <v>0.0001348524</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>25.90348172187805</v>
+        <v>25.90748167037964</v>
       </c>
       <c r="B266" t="n">
-        <v>9.250118e-09</v>
+        <v>0.0001347454</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>26.00448751449585</v>
+        <v>26.00948762893677</v>
       </c>
       <c r="B267" t="n">
-        <v>9.383446e-09</v>
+        <v>0.0001347901</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>26.10549330711365</v>
+        <v>26.10049271583557</v>
       </c>
       <c r="B268" t="n">
-        <v>9.407474e-09</v>
+        <v>0.0001347377</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>26.20549893379211</v>
+        <v>26.20049834251404</v>
       </c>
       <c r="B269" t="n">
-        <v>9.320147999999999e-09</v>
+        <v>0.0001347287</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>26.30550456047058</v>
+        <v>26.30150413513184</v>
       </c>
       <c r="B270" t="n">
-        <v>9.168532000000001e-09</v>
+        <v>0.0001346705</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>26.40651035308838</v>
+        <v>26.40250992774963</v>
       </c>
       <c r="B271" t="n">
-        <v>9.161582e-09</v>
+        <v>0.0001346892</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>26.50651621818542</v>
+        <v>26.50351572036743</v>
       </c>
       <c r="B272" t="n">
-        <v>9.198243e-09</v>
+        <v>0.0001346645</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>26.6075222492218</v>
+        <v>26.60552167892456</v>
       </c>
       <c r="B273" t="n">
-        <v>9.363667e-09</v>
+        <v>0.0001346354</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>26.70752787590027</v>
+        <v>26.70652747154236</v>
       </c>
       <c r="B274" t="n">
-        <v>9.415777e-09</v>
+        <v>0.0001346444</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>26.80753350257874</v>
+        <v>26.80853319168091</v>
       </c>
       <c r="B275" t="n">
-        <v>9.421135e-09</v>
+        <v>0.0001347406</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>26.90753936767578</v>
+        <v>26.90053844451904</v>
       </c>
       <c r="B276" t="n">
-        <v>9.445746000000001e-09</v>
+        <v>0.0001346967</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>27.008544921875</v>
+        <v>27.00054407119751</v>
       </c>
       <c r="B277" t="n">
-        <v>9.315013e-09</v>
+        <v>0.0001347903</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>27.10855078697205</v>
+        <v>27.10054969787598</v>
       </c>
       <c r="B278" t="n">
-        <v>9.154535000000001e-09</v>
+        <v>0.0001347526</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>27.20955634117126</v>
+        <v>27.20255565643311</v>
       </c>
       <c r="B279" t="n">
-        <v>9.292242999999999e-09</v>
+        <v>0.0001347942</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>27.30956220626831</v>
+        <v>27.30256152153015</v>
       </c>
       <c r="B280" t="n">
-        <v>9.360087e-09</v>
+        <v>0.0001347963</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>27.41056799888611</v>
+        <v>27.4045672416687</v>
       </c>
       <c r="B281" t="n">
-        <v>9.400023999999999e-09</v>
+        <v>0.000134839</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>27.50057291984558</v>
+        <v>27.5055730342865</v>
       </c>
       <c r="B282" t="n">
-        <v>9.328363999999999e-09</v>
+        <v>0.0001349868</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>27.60157895088196</v>
+        <v>27.60557866096497</v>
       </c>
       <c r="B283" t="n">
-        <v>9.374941000000001e-09</v>
+        <v>0.0001349466</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>27.70258474349976</v>
+        <v>27.70558452606201</v>
       </c>
       <c r="B284" t="n">
-        <v>9.413073e-09</v>
+        <v>0.0001350385</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>27.80259037017822</v>
+        <v>27.80559015274048</v>
       </c>
       <c r="B285" t="n">
-        <v>9.364867e-09</v>
+        <v>0.0001350414</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>27.90259623527527</v>
+        <v>27.90859603881836</v>
       </c>
       <c r="B286" t="n">
-        <v>9.26298e-09</v>
+        <v>0.0001350827</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>28.00360178947449</v>
+        <v>28.00860166549683</v>
       </c>
       <c r="B287" t="n">
-        <v>9.135867000000001e-09</v>
+        <v>0.0001351361</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>28.10360765457153</v>
+        <v>28.1096076965332</v>
       </c>
       <c r="B288" t="n">
-        <v>9.30124e-09</v>
+        <v>0.0001351212</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>28.20461320877075</v>
+        <v>28.20061278343201</v>
       </c>
       <c r="B289" t="n">
-        <v>9.274633999999999e-09</v>
+        <v>0.0001350986</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>28.3046190738678</v>
+        <v>28.30261874198914</v>
       </c>
       <c r="B290" t="n">
-        <v>9.367485e-09</v>
+        <v>0.0001351386</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>28.40462470054626</v>
+        <v>28.4076247215271</v>
       </c>
       <c r="B291" t="n">
-        <v>9.429781e-09</v>
+        <v>0.0001351533</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>28.50563049316406</v>
+        <v>28.50763058662415</v>
       </c>
       <c r="B292" t="n">
-        <v>9.177639e-09</v>
+        <v>0.0001352093</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>28.60663628578186</v>
+        <v>28.6096363067627</v>
       </c>
       <c r="B293" t="n">
-        <v>9.152184999999999e-09</v>
+        <v>0.0001352643</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>28.70664191246033</v>
+        <v>28.70964193344116</v>
       </c>
       <c r="B294" t="n">
-        <v>9.189208000000001e-09</v>
+        <v>0.0001352705</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>28.8076479434967</v>
+        <v>28.80064702033997</v>
       </c>
       <c r="B295" t="n">
-        <v>9.337174e-09</v>
+        <v>0.0001352389</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>28.90765380859375</v>
+        <v>28.90065288543701</v>
       </c>
       <c r="B296" t="n">
-        <v>9.333101999999999e-09</v>
+        <v>0.0001351981</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>29.00865936279297</v>
+        <v>29.00165843963623</v>
       </c>
       <c r="B297" t="n">
-        <v>9.156144999999999e-09</v>
+        <v>0.000135267</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>29.10866498947144</v>
+        <v>29.10066413879395</v>
       </c>
       <c r="B298" t="n">
-        <v>9.151855e-09</v>
+        <v>0.0001352618</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>29.20967078208923</v>
+        <v>29.20066976547241</v>
       </c>
       <c r="B299" t="n">
-        <v>9.206605999999999e-09</v>
+        <v>0.0001352459</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>29.30067586898804</v>
+        <v>29.30167579650879</v>
       </c>
       <c r="B300" t="n">
-        <v>9.322978e-09</v>
+        <v>0.0001352146</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>29.40068173408508</v>
+        <v>29.40368175506592</v>
       </c>
       <c r="B301" t="n">
-        <v>9.164814e-09</v>
+        <v>0.0001352705</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>29.50068736076355</v>
+        <v>29.50268745422363</v>
       </c>
       <c r="B302" t="n">
-        <v>9.232891999999999e-09</v>
+        <v>0.000135283</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>29.60969376564026</v>
+        <v>29.60369300842285</v>
       </c>
       <c r="B303" t="n">
-        <v>9.293965000000001e-09</v>
+        <v>0.0001352277</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>29.70069909095764</v>
+        <v>29.70569896697998</v>
       </c>
       <c r="B304" t="n">
-        <v>9.077269000000001e-09</v>
+        <v>0.0001352504</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>29.80170488357544</v>
+        <v>29.80070424079895</v>
       </c>
       <c r="B305" t="n">
-        <v>9.183193000000001e-09</v>
+        <v>0.0001351979</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>29.90171051025391</v>
+        <v>29.900710105896</v>
       </c>
       <c r="B306" t="n">
-        <v>9.233919999999999e-09</v>
+        <v>0.0001352468</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>30.00171613693237</v>
+        <v>30.00371599197388</v>
       </c>
       <c r="B307" t="n">
-        <v>9.200744e-09</v>
+        <v>0.0001352502</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>30.10272192955017</v>
+        <v>30.10672187805176</v>
       </c>
       <c r="B308" t="n">
-        <v>9.350361e-09</v>
+        <v>0.0001352267</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>30.20372772216797</v>
+        <v>30.20672750473022</v>
       </c>
       <c r="B309" t="n">
-        <v>9.204385e-09</v>
+        <v>0.0001352574</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>30.30473351478577</v>
+        <v>30.30973362922668</v>
       </c>
       <c r="B310" t="n">
-        <v>9.348052e-09</v>
+        <v>0.0001351847</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>30.40673923492432</v>
+        <v>30.40973925590515</v>
       </c>
       <c r="B311" t="n">
-        <v>9.198569e-09</v>
+        <v>0.0001352118</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>30.50774502754211</v>
+        <v>30.50974488258362</v>
       </c>
       <c r="B312" t="n">
-        <v>9.333109e-09</v>
+        <v>0.0001352284</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>30.60875105857849</v>
+        <v>30.60475015640259</v>
       </c>
       <c r="B313" t="n">
-        <v>9.062854e-09</v>
+        <v>0.0001351949</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>30.70975661277771</v>
+        <v>30.7037558555603</v>
       </c>
       <c r="B314" t="n">
-        <v>9.262275e-09</v>
+        <v>0.0001352298</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>30.80076193809509</v>
+        <v>30.8097620010376</v>
       </c>
       <c r="B315" t="n">
-        <v>9.125988e-09</v>
+        <v>0.0001352098</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>30.90176749229431</v>
+        <v>30.90476751327515</v>
       </c>
       <c r="B316" t="n">
-        <v>9.411472000000001e-09</v>
+        <v>0.0001352369</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>31.00277328491211</v>
+        <v>31.00877332687378</v>
       </c>
       <c r="B317" t="n">
-        <v>9.158037e-09</v>
+        <v>0.0001352058</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>31.10477900505066</v>
+        <v>31.10877919197083</v>
       </c>
       <c r="B318" t="n">
-        <v>9.394657000000001e-09</v>
+        <v>0.0001351537</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>31.20578503608704</v>
+        <v>31.20978498458862</v>
       </c>
       <c r="B319" t="n">
-        <v>9.098849999999999e-09</v>
+        <v>0.0001351858</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>31.30679082870483</v>
+        <v>31.30379033088684</v>
       </c>
       <c r="B320" t="n">
-        <v>9.226814999999999e-09</v>
+        <v>0.0001351433</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>31.40779662132263</v>
+        <v>31.40679621696472</v>
       </c>
       <c r="B321" t="n">
-        <v>9.355793e-09</v>
+        <v>0.0001351783</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>31.50880241394043</v>
+        <v>31.50080180168152</v>
       </c>
       <c r="B322" t="n">
-        <v>9.132951000000001e-09</v>
+        <v>0.0001350988</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>31.60980820655823</v>
+        <v>31.60780763626099</v>
       </c>
       <c r="B323" t="n">
-        <v>9.270558e-09</v>
+        <v>0.0001351607</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>31.70081329345703</v>
+        <v>31.70881342887878</v>
       </c>
       <c r="B324" t="n">
-        <v>9.319944e-09</v>
+        <v>0.0001351281</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>31.80281925201416</v>
+        <v>31.80681896209717</v>
       </c>
       <c r="B325" t="n">
-        <v>9.430306000000001e-09</v>
+        <v>0.0001350748</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>31.90382504463196</v>
+        <v>31.9038245677948</v>
       </c>
       <c r="B326" t="n">
-        <v>9.171262000000001e-09</v>
+        <v>0.0001350852</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>32.00483083724976</v>
+        <v>32.00183033943176</v>
       </c>
       <c r="B327" t="n">
-        <v>9.378654e-09</v>
+        <v>0.0001350168</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>32.10583662986755</v>
+        <v>32.10683631896973</v>
       </c>
       <c r="B328" t="n">
-        <v>9.106454e-09</v>
+        <v>0.0001349593</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>32.2078423500061</v>
+        <v>32.20984220504761</v>
       </c>
       <c r="B329" t="n">
-        <v>9.282957999999999e-09</v>
+        <v>0.0001349696</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>32.3088481426239</v>
+        <v>32.30084729194641</v>
       </c>
       <c r="B330" t="n">
-        <v>9.191757999999999e-09</v>
+        <v>0.0001348954</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>32.4098539352417</v>
+        <v>32.40585327148438</v>
       </c>
       <c r="B331" t="n">
-        <v>9.224097e-09</v>
+        <v>0.0001348423</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>32.50085926055908</v>
+        <v>32.50085878372192</v>
       </c>
       <c r="B332" t="n">
-        <v>9.195073000000001e-09</v>
+        <v>0.0001348302</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>32.60286498069763</v>
+        <v>32.60486459732056</v>
       </c>
       <c r="B333" t="n">
-        <v>9.374255e-09</v>
+        <v>0.0001347581</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>32.70487070083618</v>
+        <v>32.70787072181702</v>
       </c>
       <c r="B334" t="n">
-        <v>9.324566e-09</v>
+        <v>0.0001347941</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>32.80587649345398</v>
+        <v>32.80987644195557</v>
       </c>
       <c r="B335" t="n">
-        <v>9.077029e-09</v>
+        <v>0.0001348111</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>32.90688228607178</v>
+        <v>32.90088152885437</v>
       </c>
       <c r="B336" t="n">
-        <v>9.229598e-09</v>
+        <v>0.0001347703</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>33.00888824462891</v>
+        <v>33.0028874874115</v>
       </c>
       <c r="B337" t="n">
-        <v>9.047028999999999e-09</v>
+        <v>0.000134744</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>33.1098940372467</v>
+        <v>33.1038932800293</v>
       </c>
       <c r="B338" t="n">
-        <v>9.200117999999999e-09</v>
+        <v>0.0001347191</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>33.20089912414551</v>
+        <v>33.20389914512634</v>
       </c>
       <c r="B339" t="n">
-        <v>9.183243e-09</v>
+        <v>0.0001347124</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>33.30190491676331</v>
+        <v>33.30490493774414</v>
       </c>
       <c r="B340" t="n">
-        <v>9.337564000000001e-09</v>
+        <v>0.0001346913</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>33.4029107093811</v>
+        <v>33.40491056442261</v>
       </c>
       <c r="B341" t="n">
-        <v>9.072473e-09</v>
+        <v>0.0001347165</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>33.50491666793823</v>
+        <v>33.50591635704041</v>
       </c>
       <c r="B342" t="n">
-        <v>9.250121999999999e-09</v>
+        <v>0.0001347772</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>33.6049222946167</v>
+        <v>33.6069221496582</v>
       </c>
       <c r="B343" t="n">
-        <v>9.371919e-09</v>
+        <v>0.0001347925</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>33.70692825317383</v>
+        <v>33.7099277973175</v>
       </c>
       <c r="B344" t="n">
-        <v>9.172801e-09</v>
+        <v>0.0001348263</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>33.80793380737305</v>
+        <v>33.80993366241455</v>
       </c>
       <c r="B345" t="n">
-        <v>9.3643e-09</v>
+        <v>0.0001347982</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>33.90893959999084</v>
+        <v>33.90093898773193</v>
       </c>
       <c r="B346" t="n">
-        <v>9.023512e-09</v>
+        <v>0.0001348784</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>34.00094509124756</v>
+        <v>34.00194454193115</v>
       </c>
       <c r="B347" t="n">
-        <v>9.112077999999999e-09</v>
+        <v>0.0001348979</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>34.10195064544678</v>
+        <v>34.1019504070282</v>
       </c>
       <c r="B348" t="n">
-        <v>9.301177e-09</v>
+        <v>0.0001349531</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>34.20395660400391</v>
+        <v>34.20195603370667</v>
       </c>
       <c r="B349" t="n">
-        <v>9.072879000000001e-09</v>
+        <v>0.0001350094</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>34.30696249008179</v>
+        <v>34.30396175384521</v>
       </c>
       <c r="B350" t="n">
-        <v>9.107525e-09</v>
+        <v>0.0001349973</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
-        <v>34.40796828269958</v>
+        <v>34.40496754646301</v>
       </c>
       <c r="B351" t="n">
-        <v>9.266651000000001e-09</v>
+        <v>0.0001350805</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="n">
-        <v>34.50997400283813</v>
+        <v>34.50597333908081</v>
       </c>
       <c r="B352" t="n">
-        <v>9.104812000000001e-09</v>
+        <v>0.0001350463</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="n">
-        <v>34.60097932815552</v>
+        <v>34.60797905921936</v>
       </c>
       <c r="B353" t="n">
-        <v>9.200827e-09</v>
+        <v>0.000135071</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="n">
-        <v>34.70298504829407</v>
+        <v>34.70998525619507</v>
       </c>
       <c r="B354" t="n">
-        <v>9.293935e-09</v>
+        <v>0.0001350931</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="n">
-        <v>34.80299067497253</v>
+        <v>34.80099034309387</v>
       </c>
       <c r="B355" t="n">
-        <v>9.036996000000001e-09</v>
+        <v>0.0001351011</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="n">
-        <v>34.90499663352966</v>
+        <v>34.90299606323242</v>
       </c>
       <c r="B356" t="n">
-        <v>9.270064e-09</v>
+        <v>0.0001350819</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="n">
-        <v>35.00700235366821</v>
+        <v>35.00500178337097</v>
       </c>
       <c r="B357" t="n">
-        <v>9.111455999999999e-09</v>
+        <v>0.0001351407</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="n">
-        <v>35.10900831222534</v>
+        <v>35.10700798034668</v>
       </c>
       <c r="B358" t="n">
-        <v>8.936089e-09</v>
+        <v>0.0001350692</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="n">
-        <v>35.20201349258423</v>
+        <v>35.20701360702515</v>
       </c>
       <c r="B359" t="n">
-        <v>9.314667999999999e-09</v>
+        <v>0.0001351089</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="n">
-        <v>35.30501937866211</v>
+        <v>35.3090193271637</v>
       </c>
       <c r="B360" t="n">
-        <v>9.226834000000001e-09</v>
+        <v>0.0001349669</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="n">
-        <v>35.40802550315857</v>
+        <v>35.4000244140625</v>
       </c>
       <c r="B361" t="n">
-        <v>9.256209999999999e-09</v>
+        <v>0.0001350548</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="n">
-        <v>35.50003051757812</v>
+        <v>35.50303053855896</v>
       </c>
       <c r="B362" t="n">
-        <v>9.214476e-09</v>
+        <v>0.000135105</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="n">
-        <v>35.60303640365601</v>
+        <v>35.60503625869751</v>
       </c>
       <c r="B363" t="n">
-        <v>9.114628e-09</v>
+        <v>0.0001350401</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="n">
-        <v>35.70604252815247</v>
+        <v>35.70704221725464</v>
       </c>
       <c r="B364" t="n">
-        <v>9.041768e-09</v>
+        <v>0.0001350696</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="n">
-        <v>35.80904841423035</v>
+        <v>35.8000476360321</v>
       </c>
       <c r="B365" t="n">
-        <v>8.974511999999999e-09</v>
+        <v>0.0001350515</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="n">
-        <v>35.90205383300781</v>
+        <v>35.90205335617065</v>
       </c>
       <c r="B366" t="n">
-        <v>9.298002000000001e-09</v>
+        <v>0.0001350908</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="n">
-        <v>36.00505948066711</v>
+        <v>36.00405931472778</v>
       </c>
       <c r="B367" t="n">
-        <v>9.294797e-09</v>
+        <v>0.0001350828</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="n">
-        <v>36.10706543922424</v>
+        <v>36.105064868927</v>
       </c>
       <c r="B368" t="n">
-        <v>9.190655e-09</v>
+        <v>0.000135081</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="n">
-        <v>36.20007085800171</v>
+        <v>36.20707082748413</v>
       </c>
       <c r="B369" t="n">
-        <v>9.375073e-09</v>
+        <v>0.0001350185</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="n">
-        <v>36.30207657814026</v>
+        <v>36.30807638168335</v>
       </c>
       <c r="B370" t="n">
-        <v>9.281571999999999e-09</v>
+        <v>0.0001350292</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="n">
-        <v>36.40508246421814</v>
+        <v>36.40908217430115</v>
       </c>
       <c r="B371" t="n">
-        <v>9.245705000000001e-09</v>
+        <v>0.0001350106</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="n">
-        <v>36.50708818435669</v>
+        <v>36.50108766555786</v>
       </c>
       <c r="B372" t="n">
-        <v>9.157705e-09</v>
+        <v>0.0001350004</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="n">
-        <v>36.60009360313416</v>
+        <v>36.60509347915649</v>
       </c>
       <c r="B373" t="n">
-        <v>9.118998e-09</v>
+        <v>0.0001350006</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="n">
-        <v>36.70309948921204</v>
+        <v>36.70709919929504</v>
       </c>
       <c r="B374" t="n">
-        <v>9.272287999999999e-09</v>
+        <v>0.0001350323</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="n">
-        <v>36.80510520935059</v>
+        <v>36.80810523033142</v>
       </c>
       <c r="B375" t="n">
-        <v>9.266557000000001e-09</v>
+        <v>0.0001350126</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="n">
-        <v>36.90811109542847</v>
+        <v>36.90111041069031</v>
       </c>
       <c r="B376" t="n">
-        <v>9.213563e-09</v>
+        <v>0.0001350675</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="n">
-        <v>37.0001163482666</v>
+        <v>37.00311613082886</v>
       </c>
       <c r="B377" t="n">
-        <v>9.183484999999999e-09</v>
+        <v>0.0001350568</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="n">
-        <v>37.10312223434448</v>
+        <v>37.10412192344666</v>
       </c>
       <c r="B378" t="n">
-        <v>9.076027e-09</v>
+        <v>0.0001350648</v>
       </c>
     </row>
     <row r="379">
@@ -3457,231 +3457,231 @@
         <v>37.20512795448303</v>
       </c>
       <c r="B379" t="n">
-        <v>9.252976999999999e-09</v>
+        <v>0.0001350171</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="n">
-        <v>37.30913424491882</v>
+        <v>37.30713367462158</v>
       </c>
       <c r="B380" t="n">
-        <v>9.01981e-09</v>
+        <v>0.000135052</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="n">
-        <v>37.40113949775696</v>
+        <v>37.40813946723938</v>
       </c>
       <c r="B381" t="n">
-        <v>9.261207999999999e-09</v>
+        <v>0.0001350811</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="n">
-        <v>37.50414514541626</v>
+        <v>37.50014472007751</v>
       </c>
       <c r="B382" t="n">
-        <v>9.179096e-09</v>
+        <v>0.000135084</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="n">
-        <v>37.60715126991272</v>
+        <v>37.60115027427673</v>
       </c>
       <c r="B383" t="n">
-        <v>9.129715e-09</v>
+        <v>0.0001350693</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>37.70015645027161</v>
+        <v>37.70315647125244</v>
       </c>
       <c r="B384" t="n">
-        <v>9.264014000000001e-09</v>
+        <v>0.0001350542</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="n">
-        <v>37.80216217041016</v>
+        <v>37.80416202545166</v>
       </c>
       <c r="B385" t="n">
-        <v>9.166796e-09</v>
+        <v>0.0001350257</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="n">
-        <v>37.90616822242737</v>
+        <v>37.90616798400879</v>
       </c>
       <c r="B386" t="n">
-        <v>9.030436e-09</v>
+        <v>0.0001350569</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="n">
-        <v>38.00917410850525</v>
+        <v>38.00817370414734</v>
       </c>
       <c r="B387" t="n">
-        <v>9.124784e-09</v>
+        <v>0.0001350705</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="n">
-        <v>38.10217952728271</v>
+        <v>38.10917949676514</v>
       </c>
       <c r="B388" t="n">
-        <v>9.27832e-09</v>
+        <v>0.0001350319</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>38.2051854133606</v>
+        <v>38.20118474960327</v>
       </c>
       <c r="B389" t="n">
-        <v>9.272453999999999e-09</v>
+        <v>0.0001350561</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>38.30819129943848</v>
+        <v>38.3031907081604</v>
       </c>
       <c r="B390" t="n">
-        <v>9.225261e-09</v>
+        <v>0.0001350172</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>38.40119671821594</v>
+        <v>38.40419626235962</v>
       </c>
       <c r="B391" t="n">
-        <v>9.094274e-09</v>
+        <v>0.000135029</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>38.50420236587524</v>
+        <v>38.50620222091675</v>
       </c>
       <c r="B392" t="n">
-        <v>9.186577999999999e-09</v>
+        <v>0.0001349942</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>38.60720825195312</v>
+        <v>38.6082079410553</v>
       </c>
       <c r="B393" t="n">
-        <v>9.138945999999999e-09</v>
+        <v>0.0001349519</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>38.70021367073059</v>
+        <v>38.70021343231201</v>
       </c>
       <c r="B394" t="n">
-        <v>9.176709e-09</v>
+        <v>0.0001349539</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="n">
-        <v>38.8042197227478</v>
+        <v>38.80221915245056</v>
       </c>
       <c r="B395" t="n">
-        <v>9.075193999999999e-09</v>
+        <v>0.0001348587</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="n">
-        <v>38.90922546386719</v>
+        <v>38.90422487258911</v>
       </c>
       <c r="B396" t="n">
-        <v>9.045558e-09</v>
+        <v>0.000134831</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="n">
-        <v>39.0012309551239</v>
+        <v>39.00723099708557</v>
       </c>
       <c r="B397" t="n">
-        <v>9.134217999999999e-09</v>
+        <v>0.0001348487</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="n">
-        <v>39.10423684120178</v>
+        <v>39.11023688316345</v>
       </c>
       <c r="B398" t="n">
-        <v>9.169376e-09</v>
+        <v>0.0001348162</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="n">
-        <v>39.20724296569824</v>
+        <v>39.20124197006226</v>
       </c>
       <c r="B399" t="n">
-        <v>9.136169000000001e-09</v>
+        <v>0.0001347769</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>39.30024790763855</v>
+        <v>39.30224776268005</v>
       </c>
       <c r="B400" t="n">
-        <v>9.041486999999999e-09</v>
+        <v>0.0001347563</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="n">
-        <v>39.40325379371643</v>
+        <v>39.40325355529785</v>
       </c>
       <c r="B401" t="n">
-        <v>9.01334e-09</v>
+        <v>0.0001347693</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="n">
-        <v>39.50625991821289</v>
+        <v>39.50525951385498</v>
       </c>
       <c r="B402" t="n">
-        <v>9.08483e-09</v>
+        <v>0.000134785</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="n">
-        <v>39.60926556587219</v>
+        <v>39.60926532745361</v>
       </c>
       <c r="B403" t="n">
-        <v>9.231618e-09</v>
+        <v>0.0001347872</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>39.70227098464966</v>
+        <v>39.70927119255066</v>
       </c>
       <c r="B404" t="n">
-        <v>9.213315999999999e-09</v>
+        <v>0.000134739</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="n">
-        <v>39.80527710914612</v>
+        <v>39.81927752494812</v>
       </c>
       <c r="B405" t="n">
-        <v>9.105403999999999e-09</v>
+        <v>0.000134768</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="n">
-        <v>39.90828275680542</v>
+        <v>39.90228223800659</v>
       </c>
       <c r="B406" t="n">
-        <v>9.230212e-09</v>
+        <v>0.0001347742</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="n">
-        <v>40.00128793716431</v>
+        <v>40.00428795814514</v>
       </c>
       <c r="B407" t="n">
-        <v>9.184363e-09</v>
+        <v>0.0001348309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>